<commit_message>
Version 0.4 COUNT-CP - AL results
</commit_message>
<xml_diff>
--- a/results/merged_results.xlsx
+++ b/results/merged_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -638,34 +638,32 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>309</v>
+        <v>202</v>
       </c>
       <c r="C6" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1651</v>
+        <v>0.0338</v>
       </c>
       <c r="E6" t="n">
-        <v>2.1826</v>
+        <v>0.2392</v>
       </c>
       <c r="F6" t="n">
-        <v>51.0214</v>
+        <v>6.8288</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I6" t="n">
+        <v>13</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>mineask</t>
+          <t>countcp_al</t>
         </is>
       </c>
     </row>
@@ -676,19 +674,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>345</v>
+        <v>309</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1594</v>
+        <v>0.1651</v>
       </c>
       <c r="E7" t="n">
-        <v>1.6761</v>
+        <v>2.1826</v>
       </c>
       <c r="F7" t="n">
-        <v>54.9945</v>
+        <v>51.0214</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -703,43 +701,45 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>al</t>
+          <t>mineask</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>9sudoku</t>
+          <t>4sudoku</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17</v>
+        <v>345</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>1.2599</v>
+        <v>0.1594</v>
       </c>
       <c r="E8" t="n">
-        <v>1.6353</v>
+        <v>1.6761</v>
       </c>
       <c r="F8" t="n">
-        <v>21.4189</v>
+        <v>54.9945</v>
       </c>
       <c r="G8" t="n">
-        <v>954</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>824</v>
-      </c>
-      <c r="I8" t="n">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>pl_al</t>
+          <t>al</t>
         </is>
       </c>
     </row>
@@ -750,32 +750,32 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>1.2947</v>
+        <v>1.2599</v>
       </c>
       <c r="E9" t="n">
-        <v>8.3284</v>
+        <v>1.6353</v>
       </c>
       <c r="F9" t="n">
-        <v>33.6621</v>
+        <v>21.4189</v>
       </c>
       <c r="G9" t="n">
         <v>954</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>824</v>
       </c>
       <c r="I9" t="n">
         <v>34</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>pl_al_genacq</t>
+          <t>pl_al</t>
         </is>
       </c>
     </row>
@@ -786,32 +786,32 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C10" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0901</v>
+        <v>1.2947</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7887999999999999</v>
+        <v>8.3284</v>
       </c>
       <c r="F10" t="n">
-        <v>4.1423</v>
+        <v>33.6621</v>
       </c>
       <c r="G10" t="n">
-        <v>3</v>
+        <v>954</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>countcp_al_genacq</t>
+          <t>pl_al_genacq</t>
         </is>
       </c>
     </row>
@@ -822,34 +822,32 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="C11" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D11" t="n">
-        <v>2.5779</v>
+        <v>0.0901</v>
       </c>
       <c r="E11" t="n">
-        <v>47.6003</v>
+        <v>0.7887999999999999</v>
       </c>
       <c r="F11" t="n">
-        <v>260.3687</v>
+        <v>4.1423</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I11" t="n">
+        <v>28</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>genacq</t>
+          <t>countcp_al_genacq</t>
         </is>
       </c>
     </row>
@@ -860,19 +858,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6172</v>
+        <v>101</v>
       </c>
       <c r="C12" t="n">
-        <v>1234</v>
+        <v>36</v>
       </c>
       <c r="D12" t="n">
-        <v>0.3146</v>
+        <v>2.5779</v>
       </c>
       <c r="E12" t="n">
-        <v>6.9725</v>
+        <v>47.6003</v>
       </c>
       <c r="F12" t="n">
-        <v>1941.6964</v>
+        <v>260.3687</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
@@ -887,7 +885,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>mineask</t>
+          <t>genacq</t>
         </is>
       </c>
     </row>
@@ -898,106 +896,108 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7643</v>
+        <v>4097</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.205</v>
+        <v>0.2206</v>
       </c>
       <c r="E13" t="n">
-        <v>5.4047</v>
+        <v>1.4524</v>
       </c>
       <c r="F13" t="n">
-        <v>1567.121</v>
+        <v>903.6096</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>813</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I13" t="n">
+        <v>28</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>al</t>
+          <t>countcp_al</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>examtt_advanced</t>
+          <t>9sudoku</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2249</v>
+        <v>6172</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>1234</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3279</v>
+        <v>0.3146</v>
       </c>
       <c r="E14" t="n">
-        <v>3.3956</v>
+        <v>6.9725</v>
       </c>
       <c r="F14" t="n">
-        <v>737.4732</v>
+        <v>1941.6964</v>
       </c>
       <c r="G14" t="n">
-        <v>1319</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>828</v>
-      </c>
-      <c r="I14" t="n">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>pl_al</t>
+          <t>mineask</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>examtt_advanced</t>
+          <t>9sudoku</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6292</v>
+        <v>7643</v>
       </c>
       <c r="C15" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3069</v>
+        <v>0.205</v>
       </c>
       <c r="E15" t="n">
-        <v>4.5061</v>
+        <v>5.4047</v>
       </c>
       <c r="F15" t="n">
-        <v>1931.1836</v>
+        <v>1567.121</v>
       </c>
       <c r="G15" t="n">
-        <v>1319</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
       </c>
-      <c r="I15" t="n">
-        <v>16</v>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>pl_al_genacq</t>
+          <t>al</t>
         </is>
       </c>
     </row>
@@ -1008,34 +1008,32 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>7071</v>
+        <v>2249</v>
       </c>
       <c r="C16" t="n">
-        <v>2839</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5679999999999999</v>
+        <v>0.3279</v>
       </c>
       <c r="E16" t="n">
-        <v>13.4583</v>
+        <v>3.3956</v>
       </c>
       <c r="F16" t="n">
-        <v>4016.6227</v>
+        <v>737.4732</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1319</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>828</v>
+      </c>
+      <c r="I16" t="n">
+        <v>16</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>mineask</t>
+          <t>pl_al</t>
         </is>
       </c>
     </row>
@@ -1046,106 +1044,108 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>8922</v>
+        <v>6292</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2988</v>
+        <v>0.3069</v>
       </c>
       <c r="E17" t="n">
-        <v>5.1951</v>
+        <v>4.5061</v>
       </c>
       <c r="F17" t="n">
-        <v>2665.8468</v>
+        <v>1931.1836</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1319</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I17" t="n">
+        <v>16</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>al</t>
+          <t>pl_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>examtt_simple</t>
+          <t>examtt_advanced</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2853</v>
+        <v>7071</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>2839</v>
       </c>
       <c r="D18" t="n">
-        <v>0.292</v>
+        <v>0.5679999999999999</v>
       </c>
       <c r="E18" t="n">
-        <v>2.0752</v>
+        <v>13.4583</v>
       </c>
       <c r="F18" t="n">
-        <v>832.9482</v>
+        <v>4016.6227</v>
       </c>
       <c r="G18" t="n">
-        <v>1764</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>828</v>
-      </c>
-      <c r="I18" t="n">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>pl_al</t>
+          <t>mineask</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>examtt_simple</t>
+          <t>examtt_advanced</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>6234</v>
+        <v>8922</v>
       </c>
       <c r="C19" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2879</v>
+        <v>0.2988</v>
       </c>
       <c r="E19" t="n">
-        <v>2.1081</v>
+        <v>5.1951</v>
       </c>
       <c r="F19" t="n">
-        <v>1794.584</v>
+        <v>2665.8468</v>
       </c>
       <c r="G19" t="n">
-        <v>717</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
         <v>0</v>
       </c>
-      <c r="I19" t="n">
-        <v>40</v>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>countcp_al_genacq</t>
+          <t>al</t>
         </is>
       </c>
     </row>
@@ -1156,32 +1156,32 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>6745</v>
+        <v>2853</v>
       </c>
       <c r="C20" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3096</v>
+        <v>0.292</v>
       </c>
       <c r="E20" t="n">
-        <v>3.8026</v>
+        <v>2.0752</v>
       </c>
       <c r="F20" t="n">
-        <v>2087.9801</v>
+        <v>832.9482</v>
       </c>
       <c r="G20" t="n">
         <v>1764</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>828</v>
       </c>
       <c r="I20" t="n">
         <v>16</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>pl_al_genacq</t>
+          <t>pl_al</t>
         </is>
       </c>
     </row>
@@ -1192,34 +1192,32 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>7535</v>
+        <v>6234</v>
       </c>
       <c r="C21" t="n">
-        <v>2809</v>
+        <v>40</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5657</v>
+        <v>0.2879</v>
       </c>
       <c r="E21" t="n">
-        <v>16.0182</v>
+        <v>2.1081</v>
       </c>
       <c r="F21" t="n">
-        <v>4262.6851</v>
+        <v>1794.584</v>
       </c>
       <c r="G21" t="n">
-        <v>0</v>
+        <v>717</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I21" t="n">
+        <v>40</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>mineask</t>
+          <t>countcp_al_genacq</t>
         </is>
       </c>
     </row>
@@ -1230,93 +1228,91 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>9042</v>
+        <v>6353</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0.307</v>
+        <v>0.2598</v>
       </c>
       <c r="E22" t="n">
-        <v>5.8536</v>
+        <v>1.4814</v>
       </c>
       <c r="F22" t="n">
-        <v>2775.751</v>
+        <v>1650.5255</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>1431</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I22" t="n">
+        <v>40</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>al</t>
+          <t>countcp_al</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_16b_diverse_countcp_countcp_al_genacq</t>
+          <t>examtt_simple</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1320</v>
+        <v>6745</v>
       </c>
       <c r="C23" t="n">
+        <v>13</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.3096</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.8026</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2087.9801</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1764</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
         <v>16</v>
       </c>
-      <c r="D23" t="n">
-        <v>0.1884</v>
-      </c>
-      <c r="E23" t="n">
-        <v>1.4932</v>
-      </c>
-      <c r="F23" t="n">
-        <v>248.7365</v>
-      </c>
-      <c r="G23" t="n">
-        <v>328</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" t="n">
-        <v>18</v>
-      </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>countcp_al_genacq</t>
+          <t>pl_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_16b_diverse_custom_al</t>
+          <t>examtt_simple</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>7648</v>
+        <v>7535</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>2809</v>
       </c>
       <c r="D24" t="n">
-        <v>0.215</v>
+        <v>0.5657</v>
       </c>
       <c r="E24" t="n">
-        <v>5.4661</v>
+        <v>16.0182</v>
       </c>
       <c r="F24" t="n">
-        <v>1644.5267</v>
+        <v>4262.6851</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -1331,104 +1327,104 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>al</t>
+          <t>mineask</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_16b_diverse_custom_pl_al</t>
+          <t>examtt_simple</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>50</v>
+        <v>9042</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0648</v>
+        <v>0.307</v>
       </c>
       <c r="E25" t="n">
-        <v>0.3963</v>
+        <v>5.8536</v>
       </c>
       <c r="F25" t="n">
-        <v>3.2403</v>
+        <v>2775.751</v>
       </c>
       <c r="G25" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>810</v>
-      </c>
-      <c r="I25" t="n">
-        <v>27</v>
+        <v>0</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>pl_al</t>
+          <t>al</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_16b_diverse_genacq_genacq</t>
+          <t>greaterThansudoku_9x9_16b_diverse_countcp_countcp_al_genacq</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>300</v>
+        <v>1320</v>
       </c>
       <c r="C26" t="n">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="D26" t="n">
-        <v>1.3307</v>
+        <v>0.1884</v>
       </c>
       <c r="E26" t="n">
-        <v>40.7096</v>
+        <v>1.4932</v>
       </c>
       <c r="F26" t="n">
-        <v>399.223</v>
+        <v>248.7365</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>328</v>
       </c>
       <c r="H26" t="n">
         <v>0</v>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I26" t="n">
+        <v>18</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>genacq</t>
+          <t>countcp_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_16b_diverse_mineask_mineask</t>
+          <t>greaterThansudoku_9x9_16b_diverse_custom_al</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>6469</v>
+        <v>7648</v>
       </c>
       <c r="C27" t="n">
-        <v>1348</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0.2968</v>
+        <v>0.215</v>
       </c>
       <c r="E27" t="n">
-        <v>7.4821</v>
+        <v>5.4661</v>
       </c>
       <c r="F27" t="n">
-        <v>1919.8797</v>
+        <v>1644.5267</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
@@ -1443,66 +1439,66 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>mineask</t>
+          <t>al</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_16b_diverse_vgc_pl_al_genacq</t>
+          <t>greaterThansudoku_9x9_16b_diverse_custom_pl_al</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>716</v>
+        <v>50</v>
       </c>
       <c r="C28" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>0.2408</v>
+        <v>0.0648</v>
       </c>
       <c r="E28" t="n">
-        <v>3.4132</v>
+        <v>0.3963</v>
       </c>
       <c r="F28" t="n">
-        <v>172.3845</v>
+        <v>3.2403</v>
       </c>
       <c r="G28" t="n">
         <v>19</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>810</v>
       </c>
       <c r="I28" t="n">
         <v>27</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>pl_al_genacq</t>
+          <t>pl_al</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_24b_diverse_custom_al</t>
+          <t>greaterThansudoku_9x9_16b_diverse_genacq_genacq</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>7605</v>
+        <v>300</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="D29" t="n">
-        <v>0.2068</v>
+        <v>1.3307</v>
       </c>
       <c r="E29" t="n">
-        <v>6.8844</v>
+        <v>40.7096</v>
       </c>
       <c r="F29" t="n">
-        <v>1572.3398</v>
+        <v>399.223</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -1517,104 +1513,104 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>al</t>
+          <t>genacq</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_24b_diverse_custom_pl_al</t>
+          <t>greaterThansudoku_9x9_16b_diverse_mineask_mineask</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>94</v>
+        <v>6469</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>1348</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0493</v>
+        <v>0.2968</v>
       </c>
       <c r="E30" t="n">
-        <v>0.4063</v>
+        <v>7.4821</v>
       </c>
       <c r="F30" t="n">
-        <v>4.6297</v>
+        <v>1919.8797</v>
       </c>
       <c r="G30" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>810</v>
-      </c>
-      <c r="I30" t="n">
-        <v>27</v>
+        <v>0</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>pl_al</t>
+          <t>mineask</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_24b_diverse_genacq_genacq</t>
+          <t>greaterThansudoku_9x9_16b_diverse_vgc_pl_al_genacq</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>424</v>
+        <v>716</v>
       </c>
       <c r="C31" t="n">
-        <v>141</v>
+        <v>20</v>
       </c>
       <c r="D31" t="n">
-        <v>1.0282</v>
+        <v>0.2408</v>
       </c>
       <c r="E31" t="n">
-        <v>26.961</v>
+        <v>3.4132</v>
       </c>
       <c r="F31" t="n">
-        <v>435.9482</v>
+        <v>172.3845</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I31" t="n">
+        <v>27</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>genacq</t>
+          <t>pl_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_24b_diverse_mineask_mineask</t>
+          <t>greaterThansudoku_9x9_24b_diverse_custom_al</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>6414</v>
+        <v>7605</v>
       </c>
       <c r="C32" t="n">
-        <v>1237</v>
+        <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>0.3111</v>
+        <v>0.2068</v>
       </c>
       <c r="E32" t="n">
-        <v>7.7986</v>
+        <v>6.8844</v>
       </c>
       <c r="F32" t="n">
-        <v>1995.2028</v>
+        <v>1572.3398</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -1629,102 +1625,104 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>mineask</t>
+          <t>al</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_24b_diverse_vgc_pl_al_genacq</t>
+          <t>greaterThansudoku_9x9_24b_diverse_custom_pl_al</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3041</v>
+        <v>94</v>
       </c>
       <c r="C33" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>0.2382</v>
+        <v>0.0493</v>
       </c>
       <c r="E33" t="n">
-        <v>2.3407</v>
+        <v>0.4063</v>
       </c>
       <c r="F33" t="n">
-        <v>724.218</v>
+        <v>4.6297</v>
       </c>
       <c r="G33" t="n">
         <v>31</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>810</v>
       </c>
       <c r="I33" t="n">
         <v>27</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>pl_al_genacq</t>
+          <t>pl_al</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_8b_diverse_countcp_countcp_al_genacq</t>
+          <t>greaterThansudoku_9x9_24b_diverse_genacq_genacq</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1396</v>
+        <v>424</v>
       </c>
       <c r="C34" t="n">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="D34" t="n">
-        <v>0.1843</v>
+        <v>1.0282</v>
       </c>
       <c r="E34" t="n">
-        <v>1.4872</v>
+        <v>26.961</v>
       </c>
       <c r="F34" t="n">
-        <v>257.2749</v>
+        <v>435.9482</v>
       </c>
       <c r="G34" t="n">
-        <v>373</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
       </c>
-      <c r="I34" t="n">
-        <v>18</v>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>countcp_al_genacq</t>
+          <t>genacq</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_8b_diverse_custom_al</t>
+          <t>greaterThansudoku_9x9_24b_diverse_mineask_mineask</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>7736</v>
+        <v>6414</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>1237</v>
       </c>
       <c r="D35" t="n">
-        <v>0.1952</v>
+        <v>0.3111</v>
       </c>
       <c r="E35" t="n">
-        <v>6.104</v>
+        <v>7.7986</v>
       </c>
       <c r="F35" t="n">
-        <v>1509.7917</v>
+        <v>1995.2028</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
@@ -1739,104 +1737,102 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>al</t>
+          <t>mineask</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_8b_diverse_custom_pl_al</t>
+          <t>greaterThansudoku_9x9_24b_diverse_vgc_pl_al_genacq</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>21</v>
+        <v>3041</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0726</v>
+        <v>0.2382</v>
       </c>
       <c r="E36" t="n">
-        <v>0.6929</v>
+        <v>2.3407</v>
       </c>
       <c r="F36" t="n">
-        <v>1.5237</v>
+        <v>724.218</v>
       </c>
       <c r="G36" t="n">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="H36" t="n">
-        <v>810</v>
+        <v>0</v>
       </c>
       <c r="I36" t="n">
         <v>27</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>pl_al</t>
+          <t>pl_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_8b_diverse_genacq_genacq</t>
+          <t>greaterThansudoku_9x9_8b_diverse_countcp_countcp_al_genacq</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>199</v>
+        <v>1396</v>
       </c>
       <c r="C37" t="n">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="D37" t="n">
-        <v>1.6199</v>
+        <v>0.1843</v>
       </c>
       <c r="E37" t="n">
-        <v>30.2583</v>
+        <v>1.4872</v>
       </c>
       <c r="F37" t="n">
-        <v>322.3588</v>
+        <v>257.2749</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>373</v>
       </c>
       <c r="H37" t="n">
         <v>0</v>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I37" t="n">
+        <v>18</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>genacq</t>
+          <t>countcp_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_8b_diverse_mineask_mineask</t>
+          <t>greaterThansudoku_9x9_8b_diverse_custom_al</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>6330</v>
+        <v>7736</v>
       </c>
       <c r="C38" t="n">
-        <v>1216</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3542</v>
+        <v>0.1952</v>
       </c>
       <c r="E38" t="n">
-        <v>6.5198</v>
+        <v>6.104</v>
       </c>
       <c r="F38" t="n">
-        <v>2242.0618</v>
+        <v>1509.7917</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
@@ -1851,102 +1847,104 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>mineask</t>
+          <t>al</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_8b_diverse_vgc_pl_al_genacq</t>
+          <t>greaterThansudoku_9x9_8b_diverse_custom_pl_al</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>1260</v>
+        <v>21</v>
       </c>
       <c r="C39" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>0.245</v>
+        <v>0.0726</v>
       </c>
       <c r="E39" t="n">
-        <v>2.7521</v>
+        <v>0.6929</v>
       </c>
       <c r="F39" t="n">
-        <v>308.6891</v>
+        <v>1.5237</v>
       </c>
       <c r="G39" t="n">
         <v>11</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>810</v>
       </c>
       <c r="I39" t="n">
         <v>27</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>pl_al_genacq</t>
+          <t>pl_al</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_8b_nodiverse_countcp_countcp_al_genacq</t>
+          <t>greaterThansudoku_9x9_8b_diverse_genacq_genacq</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1065</v>
+        <v>199</v>
       </c>
       <c r="C40" t="n">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="D40" t="n">
-        <v>0.1977</v>
+        <v>1.6199</v>
       </c>
       <c r="E40" t="n">
-        <v>1.445</v>
+        <v>30.2583</v>
       </c>
       <c r="F40" t="n">
-        <v>210.5203</v>
+        <v>322.3588</v>
       </c>
       <c r="G40" t="n">
-        <v>193</v>
+        <v>0</v>
       </c>
       <c r="H40" t="n">
         <v>0</v>
       </c>
-      <c r="I40" t="n">
-        <v>18</v>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>countcp_al_genacq</t>
+          <t>genacq</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_8b_nodiverse_custom_al</t>
+          <t>greaterThansudoku_9x9_8b_diverse_mineask_mineask</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>7720</v>
+        <v>6330</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>1216</v>
       </c>
       <c r="D41" t="n">
-        <v>0.2034</v>
+        <v>0.3542</v>
       </c>
       <c r="E41" t="n">
-        <v>5.4647</v>
+        <v>6.5198</v>
       </c>
       <c r="F41" t="n">
-        <v>1569.9848</v>
+        <v>2242.0618</v>
       </c>
       <c r="G41" t="n">
         <v>0</v>
@@ -1961,104 +1959,102 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>al</t>
+          <t>mineask</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_8b_nodiverse_custom_pl_al</t>
+          <t>greaterThansudoku_9x9_8b_diverse_vgc_pl_al_genacq</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>117</v>
+        <v>1260</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D42" t="n">
-        <v>0.5422</v>
+        <v>0.245</v>
       </c>
       <c r="E42" t="n">
-        <v>7.203</v>
+        <v>2.7521</v>
       </c>
       <c r="F42" t="n">
-        <v>63.4429</v>
+        <v>308.6891</v>
       </c>
       <c r="G42" t="n">
-        <v>3883</v>
+        <v>11</v>
       </c>
       <c r="H42" t="n">
-        <v>824</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>pl_al</t>
+          <t>pl_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_8b_nodiverse_genacq_genacq</t>
+          <t>greaterThansudoku_9x9_8b_nodiverse_countcp_countcp_al_genacq</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>203</v>
+        <v>1065</v>
       </c>
       <c r="C43" t="n">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="D43" t="n">
-        <v>1.7978</v>
+        <v>0.1977</v>
       </c>
       <c r="E43" t="n">
-        <v>57.8724</v>
+        <v>1.445</v>
       </c>
       <c r="F43" t="n">
-        <v>364.9518</v>
+        <v>210.5203</v>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="H43" t="n">
         <v>0</v>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I43" t="n">
+        <v>18</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>genacq</t>
+          <t>countcp_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>greaterThansudoku_9x9_8b_nodiverse_mineask_mineask</t>
+          <t>greaterThansudoku_9x9_8b_nodiverse_custom_al</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>6496</v>
+        <v>7720</v>
       </c>
       <c r="C44" t="n">
-        <v>1678</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>0.2913</v>
+        <v>0.2034</v>
       </c>
       <c r="E44" t="n">
-        <v>8.3925</v>
+        <v>5.4647</v>
       </c>
       <c r="F44" t="n">
-        <v>1892.417</v>
+        <v>1569.9848</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
@@ -2073,115 +2069,119 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>mineask</t>
+          <t>al</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>jsudoku</t>
+          <t>greaterThansudoku_9x9_8b_nodiverse_custom_pl_al</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="C45" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0543</v>
+        <v>0.5422</v>
       </c>
       <c r="E45" t="n">
-        <v>0.7129</v>
+        <v>7.203</v>
       </c>
       <c r="F45" t="n">
-        <v>5.3751</v>
+        <v>63.4429</v>
       </c>
       <c r="G45" t="n">
-        <v>19</v>
+        <v>3883</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>824</v>
       </c>
       <c r="I45" t="n">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>countcp_al_genacq</t>
+          <t>pl_al</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>jsudoku</t>
+          <t>greaterThansudoku_9x9_8b_nodiverse_genacq_genacq</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>535</v>
+        <v>203</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D46" t="n">
-        <v>0.3397</v>
+        <v>1.7978</v>
       </c>
       <c r="E46" t="n">
-        <v>8.366400000000001</v>
+        <v>57.8724</v>
       </c>
       <c r="F46" t="n">
-        <v>181.7451</v>
+        <v>364.9518</v>
       </c>
       <c r="G46" t="n">
-        <v>1362</v>
+        <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>770</v>
-      </c>
-      <c r="I46" t="n">
-        <v>47</v>
+        <v>0</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>pl_al</t>
+          <t>genacq</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>jsudoku</t>
+          <t>greaterThansudoku_9x9_8b_nodiverse_mineask_mineask</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>619</v>
+        <v>6496</v>
       </c>
       <c r="C47" t="n">
-        <v>47</v>
+        <v>1678</v>
       </c>
       <c r="D47" t="n">
-        <v>0.3372</v>
+        <v>0.2913</v>
       </c>
       <c r="E47" t="n">
-        <v>6.8858</v>
+        <v>8.3925</v>
       </c>
       <c r="F47" t="n">
-        <v>208.7091</v>
+        <v>1892.417</v>
       </c>
       <c r="G47" t="n">
-        <v>1362</v>
+        <v>0</v>
       </c>
       <c r="H47" t="n">
         <v>0</v>
       </c>
-      <c r="I47" t="n">
-        <v>47</v>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>pl_al_genacq</t>
+          <t>mineask</t>
         </is>
       </c>
     </row>
@@ -2192,34 +2192,32 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>1526</v>
+        <v>99</v>
       </c>
       <c r="C48" t="n">
-        <v>751</v>
+        <v>18</v>
       </c>
       <c r="D48" t="n">
-        <v>0.4452</v>
+        <v>0.0543</v>
       </c>
       <c r="E48" t="n">
-        <v>19.4575</v>
+        <v>0.7129</v>
       </c>
       <c r="F48" t="n">
-        <v>679.3841</v>
+        <v>5.3751</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H48" t="n">
         <v>0</v>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I48" t="n">
+        <v>18</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>genacq</t>
+          <t>countcp_al_genacq</t>
         </is>
       </c>
     </row>
@@ -2230,34 +2228,32 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>6337</v>
+        <v>535</v>
       </c>
       <c r="C49" t="n">
-        <v>1408</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.2684</v>
+        <v>0.3397</v>
       </c>
       <c r="E49" t="n">
-        <v>6.5607</v>
+        <v>8.366400000000001</v>
       </c>
       <c r="F49" t="n">
-        <v>1700.9536</v>
+        <v>181.7451</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>1362</v>
       </c>
       <c r="H49" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>770</v>
+      </c>
+      <c r="I49" t="n">
+        <v>47</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>mineask</t>
+          <t>pl_al</t>
         </is>
       </c>
     </row>
@@ -2268,165 +2264,167 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>7676</v>
+        <v>619</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="D50" t="n">
-        <v>0.1981</v>
+        <v>0.3372</v>
       </c>
       <c r="E50" t="n">
-        <v>8.004899999999999</v>
+        <v>6.8858</v>
       </c>
       <c r="F50" t="n">
-        <v>1520.232</v>
+        <v>208.7091</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>1362</v>
       </c>
       <c r="H50" t="n">
         <v>0</v>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I50" t="n">
+        <v>47</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>al</t>
+          <t>pl_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>murder_problem</t>
+          <t>jsudoku</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>27</v>
+        <v>1526</v>
       </c>
       <c r="C51" t="n">
-        <v>4</v>
+        <v>751</v>
       </c>
       <c r="D51" t="n">
-        <v>0.0157</v>
+        <v>0.4452</v>
       </c>
       <c r="E51" t="n">
-        <v>0.1306</v>
+        <v>19.4575</v>
       </c>
       <c r="F51" t="n">
-        <v>0.4246</v>
+        <v>679.3841</v>
       </c>
       <c r="G51" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
       </c>
-      <c r="I51" t="n">
-        <v>4</v>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>countcp_al_genacq</t>
+          <t>genacq</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>murder_problem</t>
+          <t>jsudoku</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>44</v>
+        <v>3294</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>0.2874</v>
+        <v>0.2112</v>
       </c>
       <c r="E52" t="n">
-        <v>1.9153</v>
+        <v>1.4309</v>
       </c>
       <c r="F52" t="n">
-        <v>12.6462</v>
+        <v>695.8385</v>
       </c>
       <c r="G52" t="n">
-        <v>148</v>
+        <v>667</v>
       </c>
       <c r="H52" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="I52" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>pl_al</t>
+          <t>countcp_al</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>murder_problem</t>
+          <t>jsudoku</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>61</v>
+        <v>6337</v>
       </c>
       <c r="C53" t="n">
-        <v>5</v>
+        <v>1408</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1496</v>
+        <v>0.2684</v>
       </c>
       <c r="E53" t="n">
-        <v>2.4487</v>
+        <v>6.5607</v>
       </c>
       <c r="F53" t="n">
-        <v>9.1236</v>
+        <v>1700.9536</v>
       </c>
       <c r="G53" t="n">
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="H53" t="n">
         <v>0</v>
       </c>
-      <c r="I53" t="n">
-        <v>5</v>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>pl_al_genacq</t>
+          <t>mineask</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>murder_problem</t>
+          <t>jsudoku</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>319</v>
+        <v>7676</v>
       </c>
       <c r="C54" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.161</v>
+        <v>0.1981</v>
       </c>
       <c r="E54" t="n">
-        <v>2.0277</v>
+        <v>8.004899999999999</v>
       </c>
       <c r="F54" t="n">
-        <v>51.3662</v>
+        <v>1520.232</v>
       </c>
       <c r="G54" t="n">
         <v>0</v>
@@ -2441,7 +2439,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>mineask</t>
+          <t>al</t>
         </is>
       </c>
     </row>
@@ -2452,66 +2450,64 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>376</v>
+        <v>27</v>
       </c>
       <c r="C55" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D55" t="n">
-        <v>0.1524</v>
+        <v>0.0157</v>
       </c>
       <c r="E55" t="n">
-        <v>2.6418</v>
+        <v>0.1306</v>
       </c>
       <c r="F55" t="n">
-        <v>57.32</v>
+        <v>0.4246</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H55" t="n">
         <v>0</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I55" t="n">
+        <v>4</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>al</t>
+          <t>countcp_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>nurse_rostering</t>
+          <t>murder_problem</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>0.065</v>
+        <v>0.2874</v>
       </c>
       <c r="E56" t="n">
-        <v>1.1855</v>
+        <v>1.9153</v>
       </c>
       <c r="F56" t="n">
-        <v>2.404</v>
+        <v>12.6462</v>
       </c>
       <c r="G56" t="n">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="H56" t="n">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="I56" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
@@ -2522,95 +2518,95 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>nurse_rostering</t>
+          <t>murder_problem</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C57" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D57" t="n">
-        <v>0.0175</v>
+        <v>0.1496</v>
       </c>
       <c r="E57" t="n">
-        <v>0.1273</v>
+        <v>2.4487</v>
       </c>
       <c r="F57" t="n">
-        <v>0.7687</v>
+        <v>9.1236</v>
       </c>
       <c r="G57" t="n">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="H57" t="n">
         <v>0</v>
       </c>
       <c r="I57" t="n">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>countcp_al_genacq</t>
+          <t>pl_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>nurse_rostering</t>
+          <t>murder_problem</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="C58" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>0.062</v>
+        <v>0.0287</v>
       </c>
       <c r="E58" t="n">
-        <v>0.822</v>
+        <v>0.1246</v>
       </c>
       <c r="F58" t="n">
-        <v>3.6569</v>
+        <v>3.477</v>
       </c>
       <c r="G58" t="n">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="H58" t="n">
         <v>0</v>
       </c>
       <c r="I58" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>pl_al_genacq</t>
+          <t>countcp_al</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>nurse_rostering</t>
+          <t>murder_problem</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>196</v>
+        <v>319</v>
       </c>
       <c r="C59" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D59" t="n">
-        <v>0.1422</v>
+        <v>0.161</v>
       </c>
       <c r="E59" t="n">
-        <v>1.7122</v>
+        <v>2.0277</v>
       </c>
       <c r="F59" t="n">
-        <v>27.8756</v>
+        <v>51.3662</v>
       </c>
       <c r="G59" t="n">
         <v>0</v>
@@ -2632,23 +2628,23 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>nurse_rostering</t>
+          <t>murder_problem</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>201</v>
+        <v>376</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>0.1587</v>
+        <v>0.1524</v>
       </c>
       <c r="E60" t="n">
-        <v>2.8018</v>
+        <v>2.6418</v>
       </c>
       <c r="F60" t="n">
-        <v>31.8896</v>
+        <v>57.32</v>
       </c>
       <c r="G60" t="n">
         <v>0</v>
@@ -2670,68 +2666,68 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>sudoku_9x9_diverse_countcp_countcp_al_genacq</t>
+          <t>nurse_rostering</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>959</v>
+        <v>37</v>
       </c>
       <c r="C61" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>0.1835</v>
+        <v>0.065</v>
       </c>
       <c r="E61" t="n">
-        <v>1.4489</v>
+        <v>1.1855</v>
       </c>
       <c r="F61" t="n">
-        <v>175.9975</v>
+        <v>2.404</v>
       </c>
       <c r="G61" t="n">
-        <v>329</v>
+        <v>54</v>
       </c>
       <c r="H61" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="I61" t="n">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>countcp_al_genacq</t>
+          <t>pl_al</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>sudoku_9x9_nodiverse_countcp_countcp_al_genacq</t>
+          <t>nurse_rostering</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>820</v>
+        <v>44</v>
       </c>
       <c r="C62" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D62" t="n">
-        <v>0.1792</v>
+        <v>0.0175</v>
       </c>
       <c r="E62" t="n">
-        <v>1.4585</v>
+        <v>0.1273</v>
       </c>
       <c r="F62" t="n">
-        <v>146.9621</v>
+        <v>0.7687</v>
       </c>
       <c r="G62" t="n">
-        <v>162</v>
+        <v>12</v>
       </c>
       <c r="H62" t="n">
         <v>0</v>
       </c>
       <c r="I62" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
@@ -2742,97 +2738,95 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>sudoku_9x9_nodiverse_custom_al</t>
+          <t>nurse_rostering</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>7594</v>
+        <v>59</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D63" t="n">
-        <v>0.1635</v>
+        <v>0.062</v>
       </c>
       <c r="E63" t="n">
-        <v>5.1543</v>
+        <v>0.822</v>
       </c>
       <c r="F63" t="n">
-        <v>1241.3644</v>
+        <v>3.6569</v>
       </c>
       <c r="G63" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="H63" t="n">
         <v>0</v>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="I63" t="n">
+        <v>7</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>al</t>
+          <t>pl_al_genacq</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>sudoku_9x9_nodiverse_custom_pl_al</t>
+          <t>nurse_rostering</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>1.6731</v>
+        <v>0.0208</v>
       </c>
       <c r="E64" t="n">
-        <v>5.9291</v>
+        <v>0.1073</v>
       </c>
       <c r="F64" t="n">
-        <v>35.1354</v>
+        <v>1.3947</v>
       </c>
       <c r="G64" t="n">
-        <v>3854</v>
+        <v>27</v>
       </c>
       <c r="H64" t="n">
-        <v>840</v>
+        <v>0</v>
       </c>
       <c r="I64" t="n">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>pl_al</t>
+          <t>countcp_al</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>sudoku_9x9_nodiverse_genacq_genacq</t>
+          <t>nurse_rostering</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>91</v>
+        <v>196</v>
       </c>
       <c r="C65" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="D65" t="n">
-        <v>2.456</v>
+        <v>0.1422</v>
       </c>
       <c r="E65" t="n">
-        <v>21.8738</v>
+        <v>1.7122</v>
       </c>
       <c r="F65" t="n">
-        <v>223.5004</v>
+        <v>27.8756</v>
       </c>
       <c r="G65" t="n">
         <v>0</v>
@@ -2847,30 +2841,30 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>genacq</t>
+          <t>mineask</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>sudoku_9x9_nodiverse_mineask_mineask</t>
+          <t>nurse_rostering</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>6314</v>
+        <v>201</v>
       </c>
       <c r="C66" t="n">
-        <v>963</v>
+        <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>0.2447</v>
+        <v>0.1587</v>
       </c>
       <c r="E66" t="n">
-        <v>5.3293</v>
+        <v>2.8018</v>
       </c>
       <c r="F66" t="n">
-        <v>1545.1286</v>
+        <v>31.8896</v>
       </c>
       <c r="G66" t="n">
         <v>0</v>
@@ -2885,41 +2879,299 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>mineask</t>
+          <t>al</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
+          <t>sudoku_9x9_diverse_countcp_countcp_al_genacq</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>959</v>
+      </c>
+      <c r="C67" t="n">
+        <v>18</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.1835</v>
+      </c>
+      <c r="E67" t="n">
+        <v>1.4489</v>
+      </c>
+      <c r="F67" t="n">
+        <v>175.9975</v>
+      </c>
+      <c r="G67" t="n">
+        <v>329</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="n">
+        <v>18</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>countcp_al_genacq</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>sudoku_9x9_nodiverse_countcp_al_countcp_al</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>3270</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.2095</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1.5044</v>
+      </c>
+      <c r="F68" t="n">
+        <v>685.1798</v>
+      </c>
+      <c r="G68" t="n">
+        <v>648</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>18</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>countcp_al</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>sudoku_9x9_nodiverse_countcp_countcp_al_genacq</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>820</v>
+      </c>
+      <c r="C69" t="n">
+        <v>18</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.1792</v>
+      </c>
+      <c r="E69" t="n">
+        <v>1.4585</v>
+      </c>
+      <c r="F69" t="n">
+        <v>146.9621</v>
+      </c>
+      <c r="G69" t="n">
+        <v>162</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="n">
+        <v>18</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>countcp_al_genacq</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>sudoku_9x9_nodiverse_custom_al</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>7594</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.1635</v>
+      </c>
+      <c r="E70" t="n">
+        <v>5.1543</v>
+      </c>
+      <c r="F70" t="n">
+        <v>1241.3644</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>al</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>sudoku_9x9_nodiverse_custom_pl_al</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>21</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1.6731</v>
+      </c>
+      <c r="E71" t="n">
+        <v>5.9291</v>
+      </c>
+      <c r="F71" t="n">
+        <v>35.1354</v>
+      </c>
+      <c r="G71" t="n">
+        <v>3854</v>
+      </c>
+      <c r="H71" t="n">
+        <v>840</v>
+      </c>
+      <c r="I71" t="n">
+        <v>42</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>pl_al</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>sudoku_9x9_nodiverse_genacq_genacq</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>91</v>
+      </c>
+      <c r="C72" t="n">
+        <v>36</v>
+      </c>
+      <c r="D72" t="n">
+        <v>2.456</v>
+      </c>
+      <c r="E72" t="n">
+        <v>21.8738</v>
+      </c>
+      <c r="F72" t="n">
+        <v>223.5004</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>genacq</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>sudoku_9x9_nodiverse_mineask_mineask</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>6314</v>
+      </c>
+      <c r="C73" t="n">
+        <v>963</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.2447</v>
+      </c>
+      <c r="E73" t="n">
+        <v>5.3293</v>
+      </c>
+      <c r="F73" t="n">
+        <v>1545.1286</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>mineask</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
           <t>sudoku_9x9_nodiverse_vgc_pl_al_genacq</t>
         </is>
       </c>
-      <c r="B67" t="n">
+      <c r="B74" t="n">
         <v>30</v>
       </c>
-      <c r="C67" t="n">
+      <c r="C74" t="n">
         <v>42</v>
       </c>
-      <c r="D67" t="n">
+      <c r="D74" t="n">
         <v>2.321</v>
       </c>
-      <c r="E67" t="n">
+      <c r="E74" t="n">
         <v>26.4313</v>
       </c>
-      <c r="F67" t="n">
+      <c r="F74" t="n">
         <v>69.6305</v>
       </c>
-      <c r="G67" t="n">
+      <c r="G74" t="n">
         <v>3854</v>
       </c>
-      <c r="H67" t="n">
-        <v>0</v>
-      </c>
-      <c r="I67" t="n">
+      <c r="H74" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="n">
         <v>42</v>
       </c>
-      <c r="J67" t="inlineStr">
+      <c r="J74" t="inlineStr">
         <is>
           <t>pl_al_genacq</t>
         </is>

</xml_diff>